<commit_message>
V1.17.0 CRIAÇÃO DA PASTA FOTOS
</commit_message>
<xml_diff>
--- a/BODY/auxi/BODY.xlsx
+++ b/BODY/auxi/BODY.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ColdFusion2023\cfusion\wwwroot\qualidade\BODY\auxi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jefferson.teixeira\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="618">
   <si>
     <t>BARCODE</t>
   </si>
@@ -39,13 +39,7 @@
     <t>PROBLEMA</t>
   </si>
   <si>
-    <t>MODELO</t>
-  </si>
-  <si>
     <t>COLABORADOR</t>
-  </si>
-  <si>
-    <t>INTERVALO</t>
   </si>
   <si>
     <t>Peça</t>
@@ -2236,28 +2230,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="28.7109375" customWidth="1"/>
     <col min="6" max="6" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -2272,13 +2264,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>604</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
+        <v>602</v>
       </c>
     </row>
   </sheetData>
@@ -2307,229 +2293,229 @@
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="F2" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3" s="1">
         <v>4.1666666666666699E-2</v>
       </c>
       <c r="E3" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="F3" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D4" s="1">
         <v>8.3333333333333301E-2</v>
       </c>
       <c r="E4" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="F4" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D5" s="1">
         <v>0.125</v>
       </c>
       <c r="E5" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D6" s="1">
         <v>0.16666666666666699</v>
       </c>
       <c r="E6" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D7" s="1">
         <v>0.20833333333333301</v>
       </c>
       <c r="E7" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D8" s="1">
         <v>0.25</v>
       </c>
       <c r="E8" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D9" s="1">
         <v>0.29166666666666702</v>
       </c>
       <c r="E9" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D10" s="1">
         <v>0.33333333333333298</v>
       </c>
       <c r="E10" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D11" s="1">
         <v>0.375</v>
       </c>
       <c r="E11" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D12" s="1">
         <v>0.41666666666666702</v>
       </c>
       <c r="E12" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D13" s="1">
         <v>0.45833333333333298</v>
@@ -2537,13 +2523,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D14" s="1">
         <v>0.5</v>
@@ -2551,13 +2537,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D15" s="1">
         <v>0.54166666666666696</v>
@@ -2565,13 +2551,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D16" s="1">
         <v>0.58333333333333304</v>
@@ -2579,13 +2565,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D17" s="1">
         <v>0.625</v>
@@ -2593,13 +2579,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D18" s="1">
         <v>0.66666666666666696</v>
@@ -2607,13 +2593,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D19" s="1">
         <v>0.70833333333333304</v>
@@ -2621,13 +2607,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D20" s="1">
         <v>0.75</v>
@@ -2635,13 +2621,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D21" s="1">
         <v>0.79166666666666696</v>
@@ -2649,13 +2635,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D22" s="1">
         <v>0.83333333333333304</v>
@@ -2663,13 +2649,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D23" s="1">
         <v>0.875</v>
@@ -2677,13 +2663,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D24" s="1">
         <v>0.91666666666666696</v>
@@ -2691,13 +2677,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D25" s="1">
         <v>0.95833333333333304</v>
@@ -2705,2512 +2691,2512 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C31" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C32" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C33" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C34" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C35" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C38" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C39" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C40" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C41" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C42" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C43" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C44" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C45" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C46" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C47" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C48" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C49" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C50" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C51" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C52" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C53" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C54" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C55" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C56" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C57" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C58" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C59" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C60" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C61" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C62" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C63" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C64" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C65" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="109" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="129" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="130" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="131" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="132" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="133" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="134" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="135" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="136" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="138" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="139" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="140" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="141" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="142" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="143" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="144" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="145" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="146" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="147" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="148" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="149" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="150" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="151" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="152" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="153" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="154" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="155" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="156" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="157" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B157" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="158" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="159" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="160" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="161" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="162" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="163" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="164" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="165" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="166" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="167" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="168" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="169" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="170" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="171" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B171" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="172" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="173" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="174" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="175" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="176" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="177" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="178" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="179" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="180" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="181" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="182" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B182" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="183" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B183" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="184" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="185" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="186" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="187" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="188" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="189" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="190" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="191" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="192" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="193" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B193" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="194" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="195" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="196" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="197" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="198" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="199" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="200" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="201" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B201" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="202" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="203" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="204" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B204" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="205" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B205" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="206" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B206" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="207" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B207" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="208" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B208" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="209" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="210" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B210" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="211" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B211" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="212" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B212" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="213" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B213" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="214" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B214" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="215" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B215" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="216" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B216" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="217" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="218" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B218" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="219" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B219" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="220" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B220" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="221" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B221" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="222" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B222" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="223" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B223" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="224" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B224" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="225" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B225" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="226" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B226" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="227" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B227" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="228" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B228" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="229" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B229" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="230" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B230" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="231" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B231" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="232" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B232" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="233" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B233" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="234" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B234" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="235" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B235" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="236" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B236" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="237" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B237" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="238" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B238" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="239" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B239" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="240" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B240" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="241" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B241" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="242" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B242" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="243" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B243" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="244" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B244" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="245" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B245" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="246" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B246" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="247" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B247" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="248" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B248" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="249" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B249" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="250" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B250" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="251" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B251" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="252" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B252" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="253" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B253" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="254" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B254" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="255" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B255" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="256" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B256" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="257" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B257" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="258" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B258" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="259" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B259" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="260" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B260" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="261" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B261" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="262" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B262" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="263" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B263" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="264" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B264" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="265" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B265" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="266" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B266" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="267" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B267" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="268" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B268" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="269" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B269" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="270" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B270" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="271" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B271" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="272" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B272" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="273" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B273" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="274" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B274" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="275" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B275" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="276" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B276" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="277" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B277" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="278" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B278" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="279" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B279" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="280" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B280" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="281" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B281" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="282" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B282" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="283" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B283" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="284" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B284" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="285" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B285" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="286" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B286" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="287" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B287" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="288" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B288" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="289" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B289" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="290" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B290" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="291" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B291" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="292" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B292" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="293" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B293" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="294" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B294" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="295" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B295" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="296" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B296" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="297" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B297" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="298" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B298" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="299" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B299" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="300" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B300" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="301" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B301" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="302" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B302" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="303" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B303" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="304" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B304" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="305" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B305" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="306" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B306" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="307" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B307" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="308" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B308" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="309" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B309" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="310" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B310" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="311" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B311" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="312" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B312" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="313" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B313" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="314" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B314" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="315" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B315" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="316" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B316" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="317" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B317" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="318" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B318" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="319" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B319" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="320" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B320" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="321" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B321" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="322" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B322" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="323" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B323" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="324" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B324" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="325" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B325" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="326" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B326" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="327" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B327" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="328" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B328" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="329" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B329" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="330" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B330" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="331" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B331" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="332" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B332" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="333" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B333" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="334" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B334" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="335" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B335" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="336" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B336" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="337" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B337" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="338" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B338" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="339" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B339" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="340" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B340" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="341" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B341" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="342" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B342" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="343" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B343" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="344" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B344" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="345" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B345" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="346" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B346" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="347" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B347" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="348" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B348" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="349" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B349" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="350" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B350" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="351" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B351" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="352" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B352" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="353" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B353" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="354" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B354" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="355" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B355" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="356" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B356" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="357" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B357" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="358" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B358" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="359" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B359" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="360" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B360" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="361" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B361" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="362" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B362" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="363" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B363" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="364" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B364" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="365" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B365" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="366" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B366" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="367" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B367" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="368" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B368" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="369" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B369" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="370" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B370" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="371" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B371" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="372" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B372" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="373" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B373" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="374" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B374" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="375" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B375" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="376" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B376" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="377" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B377" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="378" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B378" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="379" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B379" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="380" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B380" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="381" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B381" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="382" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B382" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="383" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B383" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="384" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B384" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="385" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B385" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="386" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B386" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="387" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B387" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="388" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B388" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="389" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B389" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="390" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B390" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="391" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B391" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="392" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B392" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="393" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B393" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="394" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B394" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="395" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B395" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="396" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B396" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="397" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B397" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="398" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B398" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="399" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B399" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="400" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B400" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="401" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B401" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="402" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B402" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="403" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B403" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="404" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B404" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="405" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B405" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="406" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B406" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="407" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B407" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="408" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B408" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="409" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B409" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="410" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B410" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="411" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B411" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="412" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B412" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="413" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B413" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="414" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B414" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="415" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B415" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="416" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B416" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="417" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B417" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="418" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B418" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="419" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B419" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="420" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B420" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="421" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B421" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
     </row>
     <row r="422" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B422" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="423" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B423" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="424" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B424" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="425" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B425" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="426" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B426" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="427" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B427" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="428" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B428" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="429" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B429" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="430" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B430" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="431" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B431" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="432" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B432" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="433" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B433" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="434" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B434" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="435" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B435" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="436" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B436" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="437" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B437" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="438" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B438" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="439" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B439" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="440" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B440" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="441" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B441" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="442" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B442" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="443" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B443" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="444" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B444" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="445" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B445" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="446" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B446" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
     </row>
     <row r="447" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B447" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
     </row>
     <row r="448" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B448" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="449" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B449" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="450" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B450" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="451" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B451" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="452" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B452" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="453" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B453" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="454" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B454" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="455" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B455" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="456" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B456" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="457" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B457" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="458" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B458" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="459" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B459" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="460" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B460" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="461" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B461" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="462" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B462" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="463" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B463" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="464" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B464" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="465" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B465" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="466" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B466" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="467" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B467" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="468" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B468" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="469" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B469" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="470" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B470" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="471" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B471" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="472" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B472" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="473" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B473" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="474" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B474" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="475" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B475" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="476" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B476" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="477" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B477" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="478" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B478" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="479" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B479" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="480" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B480" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="481" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B481" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="482" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B482" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="483" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B483" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="484" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B484" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="485" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B485" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="486" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B486" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="487" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B487" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="488" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B488" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="489" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B489" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="490" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B490" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="491" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B491" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="492" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B492" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="493" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B493" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="494" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B494" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="495" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B495" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="496" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B496" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="497" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B497" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="498" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B498" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="499" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B499" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="500" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B500" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>